<commit_message>
decrease the bus capacitors to 1e-8.
Generalized eig() can produce the correct eigenvalues.
</commit_message>
<xml_diff>
--- a/CustomerData3.xlsx
+++ b/CustomerData3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2821631C-92AD-4691-BF37-141974C52F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670D5B71-F5D1-4578-A2A0-EDD512F9CF98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2307,7 +2307,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>1E-10</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0.20912</v>
@@ -2330,7 +2330,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>1E-10</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0.55618000000000001</v>
@@ -2353,7 +2353,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="1">
-        <v>1E-10</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0.25202000000000002</v>
@@ -2445,7 +2445,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1">
-        <v>1E-10</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0.17615</v>
@@ -2468,7 +2468,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="1">
-        <v>1E-10</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0.11001</v>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2750,7 +2750,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>1E-10</v>
+        <v>0.19</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>1E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="F44">
         <v>0</v>

</xml_diff>